<commit_message>
add access to mysql database
</commit_message>
<xml_diff>
--- a/OrderForm.xlsx
+++ b/OrderForm.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>[Company Name]</t>
   </si>
@@ -41,12 +41,6 @@
     <t>[City, ST  ZIP]</t>
   </si>
   <si>
-    <t>[Name]</t>
-  </si>
-  <si>
-    <t>[Phone]</t>
-  </si>
-  <si>
     <t>SHIP VIA</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>OTHER</t>
   </si>
   <si>
-    <t>[Name, Phone #, E-mail]</t>
-  </si>
-  <si>
     <t>DATE</t>
   </si>
   <si>
@@ -168,6 +159,12 @@
   </si>
   <si>
     <t>https://www.vertex42.com/licensing/EULA_privateuse.html</t>
+  </si>
+  <si>
+    <t>Shouran Mu</t>
+  </si>
+  <si>
+    <t>ABC</t>
   </si>
 </sst>
 </file>
@@ -574,7 +571,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -712,37 +709,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="55"/>
-      </left>
-      <right style="thin">
-        <color indexed="55"/>
-      </right>
-      <top style="thin">
-        <color indexed="55"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0"/>
       </left>
@@ -1041,6 +1007,82 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="55"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="55"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="55"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1093,7 +1135,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="9" fillId="0" fontId="21" numFmtId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="84">
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
@@ -1102,21 +1144,21 @@
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="15" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="16" fillId="0" fontId="33" numFmtId="0" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="12" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="13" fillId="0" fontId="33" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="15" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="17" fillId="0" fontId="23" numFmtId="0" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="12" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="14" fillId="0" fontId="23" numFmtId="0" xfId="0">
       <alignment horizontal="left" indent="1" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="15" fillId="0" fontId="23" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="12" fillId="0" fontId="23" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="15" fillId="0" fontId="24" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="12" fillId="0" fontId="24" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="15" fillId="0" fontId="23" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="12" fillId="0" fontId="23" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
@@ -1129,15 +1171,6 @@
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="11" fillId="0" fontId="27" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="12" fillId="0" fontId="27" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1150,52 +1183,40 @@
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="11" fillId="0" fontId="32" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="13" fillId="21" fontId="28" numFmtId="164" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="7" fillId="0" fontId="27" numFmtId="165" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="14" fillId="0" fontId="27" numFmtId="165" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="11" fillId="20" fontId="27" numFmtId="165" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="15" fillId="0" fontId="23" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="12" fillId="0" fontId="23" numFmtId="0" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="right" indent="1" vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="22" fontId="29" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="30" fillId="22" fontId="29" numFmtId="10" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="27" fillId="22" fontId="29" numFmtId="10" xfId="0">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="30" fillId="22" fontId="29" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="27" fillId="22" fontId="29" numFmtId="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="33" fillId="0" fontId="27" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="30" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="33" fillId="20" fontId="27" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="30" fillId="20" fontId="27" numFmtId="165" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="31" fillId="22" fontId="29" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="28" fillId="22" fontId="29" numFmtId="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="32" fillId="22" fontId="29" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="29" fillId="22" fontId="29" numFmtId="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="35"/>
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="15" fillId="0" fontId="35" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="12" fillId="0" fontId="35" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="true" borderId="15" fillId="0" fontId="15" numFmtId="0" xfId="35">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="true" borderId="12" fillId="0" fontId="15" numFmtId="0" xfId="35">
       <alignment horizontal="left" wrapText="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="36" numFmtId="0" xfId="0"/>
@@ -1210,19 +1231,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="true" borderId="0" fillId="0" fontId="37" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="18" fillId="0" fontId="27" numFmtId="14" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="15" fillId="0" fontId="27" numFmtId="14" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="18" fillId="0" fontId="27" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="15" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="33" fillId="0" fontId="27" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="30" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="33" fillId="0" fontId="27" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="30" fillId="0" fontId="27" numFmtId="165" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="true" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0">
@@ -1231,24 +1252,87 @@
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="22" fontId="29" numFmtId="0" xfId="0">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="true" borderId="15" fillId="0" fontId="25" numFmtId="0" xfId="35">
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="true" borderId="12" fillId="0" fontId="25" numFmtId="0" xfId="35">
       <alignment horizontal="left" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="37" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="38" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="39" fillId="20" fontId="27" numFmtId="165" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="40" fillId="0" fontId="27" numFmtId="165" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="42" fillId="0" fontId="27" numFmtId="165" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="41" fillId="0" fontId="28" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="41" fillId="21" fontId="28" numFmtId="164" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="31" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="32" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="33" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="28" fillId="22" fontId="29" numFmtId="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="29" fillId="22" fontId="29" numFmtId="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="34" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="35" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="36" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="28" fillId="22" fontId="29" numFmtId="10" xfId="0">
+      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="19" fillId="23" fontId="30" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="16" fillId="23" fontId="30" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="20" fillId="23" fontId="30" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="17" fillId="23" fontId="30" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="21" fillId="23" fontId="30" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="18" fillId="23" fontId="30" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="19" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="20" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="21" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="22" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="23" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1258,50 +1342,23 @@
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="25" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="26" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="27" fillId="0" fontId="27" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="28" fillId="0" fontId="27" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="29" fillId="0" fontId="27" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="34" fillId="0" fontId="27" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="35" fillId="0" fontId="27" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="36" fillId="0" fontId="27" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="31" fillId="22" fontId="29" numFmtId="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="32" fillId="22" fontId="29" numFmtId="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="37" fillId="0" fontId="27" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="38" fillId="0" fontId="27" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="39" fillId="0" fontId="27" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" applyProtection="false" borderId="31" fillId="22" fontId="29" numFmtId="10" xfId="0">
-      <alignment horizontal="center" shrinkToFit="true" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1778,48 +1835,48 @@
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView showGridLines="false" tabSelected="true" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView showGridLines="false" tabSelected="true" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.9"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="39" width="16.7109375"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="39" width="11.42578125"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="39" width="11.28515625"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="4" min="4" style="39" width="16.7109375"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="5" min="5" style="39" width="11.7109375"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="39" width="12.7109375"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="7" min="7" style="39" width="14.140625"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="8" min="8" style="39" width="6.42578125"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="9" min="9" style="39" width="24.140625"/>
-    <col collapsed="false" hidden="false" max="16384" min="10" style="39" width="8.85546875"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="32" width="14.85546875"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="32" width="11.42578125"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="32" width="11.28515625"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="4" min="4" style="32" width="16.7109375"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="5" min="5" style="32" width="11.7109375"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="32" width="12.7109375"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="7" min="7" style="32" width="14.140625"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="8" min="8" style="32" width="6.42578125"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="9" min="9" style="32" width="24.140625"/>
+    <col collapsed="false" hidden="false" max="16384" min="10" style="32" width="8.85546875"/>
   </cols>
   <sheetData>
     <row ht="36.4" r="1" spans="1:9">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="21" t="s">
-        <v>23</v>
+      <c r="G1" s="18" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
-      <c r="F2" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="48">
+      <c r="F2" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="41">
         <f>TODAY()</f>
         <v>43415</v>
       </c>
@@ -1833,17 +1890,17 @@
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="49" t="s">
+      <c r="F3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="38"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="53" t="s">
-        <v>31</v>
+      <c r="A4" s="46" t="s">
+        <v>28</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -1851,11 +1908,11 @@
       <c r="E4" s="15"/>
       <c r="F4" s="5"/>
       <c r="G4" s="15"/>
-      <c r="I4" s="43"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="53" t="s">
-        <v>32</v>
+      <c r="A5" s="46" t="s">
+        <v>29</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1863,11 +1920,11 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
-      <c r="I5" s="45"/>
+      <c r="I5" s="38"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="22" t="s">
-        <v>22</v>
+      <c r="A6" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
@@ -1875,7 +1932,7 @@
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
-      <c r="I6" s="45"/>
+      <c r="I6" s="38"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="15"/>
@@ -1885,102 +1942,98 @@
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
-      <c r="I7" s="43"/>
+      <c r="I7" s="36"/>
     </row>
     <row customHeight="true" ht="18" r="8" spans="1:9">
-      <c r="A8" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="E8" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="I8" s="44"/>
+      <c r="A8" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="E8" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="15"/>
-      <c r="I9" s="45"/>
+      <c r="E9" s="79" t="str">
+        <v>Bank of China</v>
+      </c>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="I9" s="38"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
+      <c r="A10" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="15"/>
-      <c r="I10" s="45"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
+      <c r="A11" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="15"/>
-      <c r="E11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="15"/>
-      <c r="I11" s="42"/>
+      <c r="E11" s="80" t="str">
+        <v>Bockenheimer Landstraße 24, 60323 Frankfurt am Main</v>
+      </c>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="I12" s="45"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
+      <c r="A13" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="15"/>
-      <c r="E13" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="I13" s="45"/>
+      <c r="E13" s="74" t="str">
+        <v>691700900</v>
+      </c>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="I13" s="38"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
+      <c r="A14" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
       <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="I14" s="42"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="I14" s="35"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="15"/>
@@ -1990,35 +2043,35 @@
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
-      <c r="I15" s="42"/>
+      <c r="I15" s="35"/>
     </row>
     <row customHeight="true" ht="18" r="16" spans="1:9">
-      <c r="A16" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="73" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="73"/>
-      <c r="G16" s="74"/>
-      <c r="I16" s="43"/>
+      <c r="A16" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="59"/>
+      <c r="D16" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
+      <c r="I16" s="36"/>
     </row>
     <row customHeight="true" ht="18" r="17" spans="1:9">
       <c r="A17" s="14"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="76"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="62"/>
       <c r="D17" s="14"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="76"/>
-      <c r="I17" s="46"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="62"/>
+      <c r="I17" s="39"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="16"/>
@@ -2028,401 +2081,401 @@
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
-      <c r="I18" s="43"/>
+      <c r="I18" s="36"/>
     </row>
     <row customHeight="true" ht="18" r="19" spans="1:9">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="78" t="s">
+      <c r="F19" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="36" t="s">
+      <c r="G19" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="43"/>
+      <c r="I19" s="36"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="33">
+      <c r="A20" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="57"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="26">
         <v>15</v>
       </c>
-      <c r="F20" s="52">
+      <c r="F20" s="45">
         <v>150</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="27">
         <f>E20*F20</f>
         <v>2250</v>
       </c>
-      <c r="I20" s="46"/>
+      <c r="I20" s="39"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="33">
+      <c r="A21" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="57"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="26">
         <v>1</v>
       </c>
-      <c r="F21" s="52">
+      <c r="F21" s="45">
         <v>75</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="27">
         <f t="shared" ref="G21:G37" si="0">E21*F21</f>
         <v>75</v>
       </c>
-      <c r="I21" s="43"/>
+      <c r="I21" s="36"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="51"/>
-      <c r="B22" s="70"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="34">
+      <c r="A22" s="44"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22" s="43"/>
+      <c r="I22" s="36"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="51"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="34">
+      <c r="A23" s="44"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="43"/>
+      <c r="I23" s="36"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="34">
+      <c r="A24" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="56"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I24" s="43"/>
+      <c r="I24" s="36"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="70"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="34">
+      <c r="A25" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="56"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I25" s="43"/>
+      <c r="I25" s="36"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="70"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="34">
+      <c r="A26" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="56"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I26" s="43"/>
+      <c r="I26" s="36"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="70"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="34">
+      <c r="A27" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="56"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27" s="43"/>
+      <c r="I27" s="36"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="70"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="34">
+      <c r="A28" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="56"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I28" s="43"/>
+      <c r="I28" s="36"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="34">
+      <c r="A29" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="56"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29" s="43"/>
+      <c r="I29" s="36"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="34">
+      <c r="A30" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="56"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I30" s="43"/>
+      <c r="I30" s="36"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="70"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="34">
+      <c r="A31" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="56"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I31" s="43"/>
+      <c r="I31" s="36"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="70"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="34">
+      <c r="A32" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="56"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I32" s="43"/>
+      <c r="I32" s="36"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="70"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="34">
+      <c r="A33" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="56"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I33" s="43"/>
+      <c r="I33" s="36"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="70"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="34">
+      <c r="A34" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="56"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I34" s="43"/>
+      <c r="I34" s="36"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="70"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="34">
+      <c r="A35" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="56"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I35" s="43"/>
+      <c r="I35" s="36"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="70"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="34">
+      <c r="A36" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="56"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I36" s="43"/>
+      <c r="I36" s="36"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="70"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="34">
+      <c r="A37" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="56"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="43"/>
+      <c r="I37" s="36"/>
     </row>
     <row customHeight="true" ht="18" r="38" spans="1:9">
-      <c r="A38" s="69"/>
-      <c r="B38" s="69"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="27">
+      <c r="A38" s="65"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="51">
         <f>SUM(G20:G37)</f>
         <v>2325</v>
       </c>
-      <c r="I38" s="43"/>
+      <c r="I38" s="36"/>
     </row>
     <row customHeight="true" ht="18" r="39" spans="1:9">
-      <c r="A39" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="58"/>
-      <c r="C39" s="58"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="25">
+      <c r="A39" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="52">
         <v>0</v>
       </c>
-      <c r="I39" s="46"/>
+      <c r="I39" s="39"/>
     </row>
     <row customHeight="true" ht="18" r="40" spans="1:9">
-      <c r="A40" s="60"/>
-      <c r="B40" s="61"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="62"/>
+      <c r="A40" s="70"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="72"/>
       <c r="E40" s="16"/>
-      <c r="F40" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G40" s="25">
+      <c r="F40" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="52">
         <v>0</v>
       </c>
-      <c r="I40" s="46"/>
-    </row>
-    <row customHeight="true" ht="18" r="41" spans="1:9" thickBot="true">
-      <c r="A41" s="63"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="65"/>
+      <c r="I40" s="39"/>
+    </row>
+    <row customHeight="true" ht="18" r="41" spans="1:9">
+      <c r="A41" s="73"/>
+      <c r="B41" s="74"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="75"/>
       <c r="E41" s="16"/>
-      <c r="F41" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" s="26">
+      <c r="F41" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="53">
         <v>0</v>
       </c>
-      <c r="I41" s="47"/>
-    </row>
-    <row customHeight="true" ht="18" r="42" spans="1:9" thickTop="true">
-      <c r="A42" s="63"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="65"/>
+      <c r="I41" s="40"/>
+    </row>
+    <row customHeight="true" ht="18" r="42" spans="1:9">
+      <c r="A42" s="73"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="74"/>
+      <c r="D42" s="75"/>
       <c r="E42" s="16"/>
-      <c r="F42" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="24">
+      <c r="F42" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="55">
         <f>SUM(G38:G41)</f>
         <v>2325</v>
       </c>
-      <c r="I42" s="46"/>
+      <c r="I42" s="39"/>
     </row>
     <row customHeight="true" ht="18" r="43" spans="1:9">
-      <c r="A43" s="63"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="65"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="74"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="75"/>
       <c r="E43" s="16"/>
     </row>
     <row customHeight="true" ht="18" r="44" spans="1:9">
-      <c r="A44" s="66"/>
-      <c r="B44" s="67"/>
-      <c r="C44" s="67"/>
-      <c r="D44" s="68"/>
+      <c r="A44" s="76"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="78"/>
       <c r="E44" s="16"/>
     </row>
     <row r="45" spans="1:9">
       <c r="E45" s="16"/>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
-      <c r="I45" s="43"/>
+      <c r="I45" s="36"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="15"/>
@@ -2432,37 +2485,60 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
-      <c r="I46" s="43"/>
+      <c r="I46" s="36"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="B47" s="56"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="I47" s="43"/>
+      <c r="A47" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="66"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="66"/>
+      <c r="F47" s="66"/>
+      <c r="G47" s="66"/>
+      <c r="I47" s="36"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="56" t="str">
-        <v>[shouran]</v>
-      </c>
-      <c r="B48" s="56"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="I48" s="43"/>
+      <c r="A48" s="66" t="str">
+        <v>Shouran Mu</v>
+      </c>
+      <c r="B48" s="66"/>
+      <c r="C48" s="66"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="66"/>
+      <c r="I48" s="36"/>
     </row>
     <row r="49" spans="9:9">
       <c r="I49" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="35">
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E11:G12"/>
+    <mergeCell ref="E9:G10"/>
+    <mergeCell ref="A47:G47"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="E16:G16"/>
@@ -2475,26 +2551,6 @@
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="A47:G47"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
   </mergeCells>
   <printOptions horizontalCentered="true"/>
   <pageMargins bottom="0.5" footer="0.3" header="0.3" left="0.5" right="0.5" top="0.5"/>
@@ -2518,7 +2574,7 @@
     <row r="1" spans="1:3" ht="32.1" customHeight="1">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" s="8"/>
     </row>
@@ -2529,15 +2585,15 @@
     </row>
     <row r="3" spans="1:3" ht="15.4">
       <c r="A3" s="6"/>
-      <c r="B3" s="28" t="s">
-        <v>19</v>
+      <c r="B3" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6"/>
-      <c r="B4" s="41" t="s">
-        <v>44</v>
+      <c r="B4" s="34" t="s">
+        <v>41</v>
       </c>
       <c r="C4" s="8"/>
     </row>
@@ -2549,7 +2605,7 @@
     <row r="6" spans="1:3" ht="15.4">
       <c r="A6" s="6"/>
       <c r="B6" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="8"/>
     </row>
@@ -2561,7 +2617,7 @@
     <row r="8" spans="1:3" ht="30.4">
       <c r="A8" s="6"/>
       <c r="B8" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" s="8"/>
     </row>
@@ -2573,7 +2629,7 @@
     <row r="10" spans="1:3" ht="30.4">
       <c r="A10" s="6"/>
       <c r="B10" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="8"/>
     </row>
@@ -2585,7 +2641,7 @@
     <row r="12" spans="1:3" ht="30.4">
       <c r="A12" s="6"/>
       <c r="B12" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="8"/>
     </row>
@@ -2596,8 +2652,8 @@
     </row>
     <row r="14" spans="1:3" ht="15.4">
       <c r="A14" s="6"/>
-      <c r="B14" s="55" t="s">
-        <v>45</v>
+      <c r="B14" s="48" t="s">
+        <v>42</v>
       </c>
       <c r="C14" s="8"/>
     </row>
@@ -2608,8 +2664,8 @@
     </row>
     <row r="16" spans="1:3" ht="15.4">
       <c r="A16" s="6"/>
-      <c r="B16" s="40" t="s">
-        <v>34</v>
+      <c r="B16" s="33" t="s">
+        <v>31</v>
       </c>
       <c r="C16" s="8"/>
     </row>

</xml_diff>